<commit_message>
Objective function adapted + minor changes
</commit_message>
<xml_diff>
--- a/Model_formulation/00_nomenclature_definition.xlsx
+++ b/Model_formulation/00_nomenclature_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0093836\Box Sync\My Webspace\Post-doc\Spine\WP3\model\Equations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0093836\Box Sync\My Webspace\Post-doc\Spine\WP3\model\Model_formulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="212">
   <si>
     <t>latexcommand</t>
   </si>
@@ -372,9 +372,6 @@
     <t>\pUnitCapacity</t>
   </si>
   <si>
-    <t>\unit,Cdcg</t>
-  </si>
-  <si>
     <t>p^{UnitCapacity}_{#1}</t>
   </si>
   <si>
@@ -649,6 +646,18 @@
   </si>
   <si>
     <t>p_operational_cost</t>
+  </si>
+  <si>
+    <t>Capacity defining commodity group</t>
+  </si>
+  <si>
+    <t>\Cdcg</t>
+  </si>
+  <si>
+    <t>Cdcg_{#1}</t>
+  </si>
+  <si>
+    <t>Set of commodities of which the sum of the flows are restricted by the capacity of the unit</t>
   </si>
 </sst>
 </file>
@@ -1194,8 +1203,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q259" totalsRowShown="0">
-  <autoFilter ref="A1:Q259"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q260" totalsRowShown="0">
+  <autoFilter ref="A1:Q260"/>
   <sortState ref="A2:O136">
     <sortCondition ref="D1:D136"/>
   </sortState>
@@ -1485,11 +1494,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q259"/>
+  <dimension ref="A1:Q260"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1613,10 +1622,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" t="s">
         <v>165</v>
-      </c>
-      <c r="D4" t="s">
-        <v>166</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>
@@ -1659,13 +1668,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" t="s">
         <v>184</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>185</v>
-      </c>
-      <c r="F6" t="s">
-        <v>186</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1740,16 +1749,16 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" t="s">
         <v>167</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" t="s">
         <v>168</v>
-      </c>
-      <c r="F9" t="s">
-        <v>174</v>
-      </c>
-      <c r="G9" t="s">
-        <v>169</v>
       </c>
       <c r="I9" t="s">
         <v>32</v>
@@ -1769,16 +1778,16 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" t="s">
         <v>170</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
+        <v>172</v>
+      </c>
+      <c r="G10" t="s">
         <v>171</v>
-      </c>
-      <c r="F10" t="s">
-        <v>173</v>
-      </c>
-      <c r="G10" t="s">
-        <v>172</v>
       </c>
       <c r="I10" t="s">
         <v>32</v>
@@ -1827,19 +1836,19 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" t="s">
         <v>180</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
+        <v>201</v>
+      </c>
+      <c r="G12" t="s">
         <v>181</v>
       </c>
-      <c r="F12" t="s">
-        <v>202</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>182</v>
-      </c>
-      <c r="I12" t="s">
-        <v>183</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -1856,19 +1865,19 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>208</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>209</v>
       </c>
       <c r="E13" t="s">
         <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>210</v>
       </c>
       <c r="G13" t="s">
-        <v>70</v>
+        <v>211</v>
       </c>
       <c r="I13" t="s">
         <v>64</v>
@@ -1888,19 +1897,19 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
         <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I14" t="s">
         <v>64</v>
@@ -1920,22 +1929,22 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>175</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>176</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
-        <v>190</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>177</v>
+        <v>66</v>
       </c>
       <c r="G15" t="s">
-        <v>178</v>
+        <v>71</v>
       </c>
       <c r="I15" t="s">
-        <v>179</v>
+        <v>64</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1949,25 +1958,25 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="D16" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>189</v>
       </c>
       <c r="F16" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="G16" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="I16" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1984,22 +1993,22 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>156</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="I17" t="s">
-        <v>69</v>
+        <v>159</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -2016,22 +2025,22 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I18" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -2048,22 +2057,22 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="I19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -2080,22 +2089,22 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="I20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -2112,19 +2121,19 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="E21" t="s">
         <v>57</v>
       </c>
       <c r="F21" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="I21" t="s">
         <v>59</v>
@@ -2144,19 +2153,19 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
         <v>57</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I22" t="s">
         <v>59</v>
@@ -2176,22 +2185,22 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="E23" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="G23" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="I23" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2208,19 +2217,19 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D24" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F24" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G24" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="I24" t="s">
         <v>111</v>
@@ -2240,19 +2249,19 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="E25" t="s">
         <v>34</v>
       </c>
       <c r="F25" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="G25" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="I25" t="s">
         <v>111</v>
@@ -2272,19 +2281,19 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E26" t="s">
         <v>34</v>
       </c>
       <c r="F26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G26" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I26" t="s">
         <v>111</v>
@@ -2304,22 +2313,22 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D27" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E27" t="s">
-        <v>149</v>
+        <v>34</v>
       </c>
       <c r="F27" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G27" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="I27" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -2336,22 +2345,22 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F28" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G28" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2368,22 +2377,22 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D29" t="s">
+        <v>143</v>
+      </c>
+      <c r="E29" t="s">
         <v>148</v>
       </c>
-      <c r="E29" t="s">
-        <v>149</v>
-      </c>
       <c r="F29" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G29" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="I29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -2400,22 +2409,22 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D30" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E30" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" t="s">
         <v>149</v>
-      </c>
-      <c r="F30" t="s">
-        <v>153</v>
       </c>
       <c r="G30" t="s">
         <v>154</v>
       </c>
       <c r="I30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -2432,22 +2441,22 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>204</v>
+        <v>150</v>
       </c>
       <c r="D31" t="s">
-        <v>203</v>
+        <v>151</v>
       </c>
       <c r="E31" t="s">
-        <v>205</v>
+        <v>148</v>
       </c>
       <c r="F31" t="s">
-        <v>206</v>
+        <v>152</v>
       </c>
       <c r="G31" t="s">
-        <v>207</v>
+        <v>153</v>
       </c>
       <c r="I31" t="s">
-        <v>208</v>
+        <v>141</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -2464,22 +2473,22 @@
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="D32" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="E32" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="F32" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="G32" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="I32" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -2493,25 +2502,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="D33" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="E33" t="s">
-        <v>67</v>
+        <v>189</v>
       </c>
       <c r="F33" t="s">
-        <v>162</v>
+        <v>188</v>
       </c>
       <c r="G33" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="I33" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -2528,22 +2537,22 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>103</v>
+        <v>196</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="E34" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="F34" t="s">
-        <v>81</v>
+        <v>161</v>
       </c>
       <c r="G34" t="s">
-        <v>51</v>
+        <v>162</v>
       </c>
       <c r="I34" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -2560,22 +2569,22 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
       <c r="E35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F35" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="G35" t="s">
-        <v>199</v>
+        <v>51</v>
       </c>
       <c r="I35" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -2592,22 +2601,22 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E36" t="s">
         <v>49</v>
       </c>
       <c r="F36" t="s">
+        <v>122</v>
+      </c>
+      <c r="G36" t="s">
+        <v>198</v>
+      </c>
+      <c r="I36" t="s">
         <v>124</v>
-      </c>
-      <c r="G36" t="s">
-        <v>200</v>
-      </c>
-      <c r="I36" t="s">
-        <v>125</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -2624,22 +2633,22 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D37" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="E37" t="s">
         <v>49</v>
       </c>
       <c r="F37" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="G37" t="s">
-        <v>107</v>
+        <v>199</v>
       </c>
       <c r="I37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J37">
         <v>1</v>
@@ -2656,22 +2665,22 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="E38" t="s">
         <v>49</v>
       </c>
       <c r="F38" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="G38" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="I38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -2688,22 +2697,22 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="D39" t="s">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="E39" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F39" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="G39" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="I39" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="J39">
         <v>1</v>
@@ -2720,50 +2729,74 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" t="s">
+        <v>80</v>
+      </c>
+      <c r="G40" t="s">
+        <v>72</v>
+      </c>
+      <c r="I40" t="s">
+        <v>87</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>191</v>
+      </c>
+      <c r="D41" t="s">
         <v>192</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E41" t="s">
         <v>193</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F41" t="s">
         <v>194</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G41" t="s">
+        <v>197</v>
+      </c>
+      <c r="I41" t="s">
         <v>195</v>
       </c>
-      <c r="G40" t="s">
-        <v>198</v>
-      </c>
-      <c r="I40" t="s">
-        <v>196</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
-      <c r="L40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E102" s="1"/>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A238" t="s">
-        <v>14</v>
-      </c>
-      <c r="C238" t="s">
-        <v>22</v>
-      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E103" s="1"/>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C239" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
@@ -2771,7 +2804,7 @@
         <v>8</v>
       </c>
       <c r="C240" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.35">
@@ -2779,36 +2812,39 @@
         <v>8</v>
       </c>
       <c r="C241" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C242" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C243" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C244" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="C245" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.35">
@@ -2878,6 +2914,11 @@
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More on bounds + adaptation of sets
</commit_message>
<xml_diff>
--- a/Model_formulation/00_nomenclature_definition.xlsx
+++ b/Model_formulation/00_nomenclature_definition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="17970" windowHeight="5930"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="17970" windowHeight="5925"/>
   </bookViews>
   <sheets>
     <sheet name="00_nomenclature_definition" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="241">
   <si>
     <t>latexcommand</t>
   </si>
@@ -174,9 +174,6 @@
     <t>\unit,\timestep</t>
   </si>
   <si>
-    <t>\commodity,\unit,in/out,\timestep</t>
-  </si>
-  <si>
     <t>Commodity flow in/out a certain unit in a given time step</t>
   </si>
   <si>
@@ -207,24 +204,9 @@
     <t>p_tech_general</t>
   </si>
   <si>
-    <t>Output commodities of a specific unit</t>
-  </si>
-  <si>
-    <t>OutputCommodities_{#1}</t>
-  </si>
-  <si>
-    <t>\commodity,\unit</t>
-  </si>
-  <si>
     <t>s_topology</t>
   </si>
   <si>
-    <t>Input commodities of a specific unit</t>
-  </si>
-  <si>
-    <t>InputCommodities_{#1}</t>
-  </si>
-  <si>
     <t>\commodity,\timestep</t>
   </si>
   <si>
@@ -234,12 +216,6 @@
     <t>p_system</t>
   </si>
   <si>
-    <t>Set of units \unit having output commodity \commodity</t>
-  </si>
-  <si>
-    <t>Set of units \unit having input commodity  \commodity</t>
-  </si>
-  <si>
     <t>Installed capacity of a certain unit</t>
   </si>
   <si>
@@ -288,12 +264,6 @@
     <t>v_investment</t>
   </si>
   <si>
-    <t>\OutputCommodities</t>
-  </si>
-  <si>
-    <t>\InputCommodities</t>
-  </si>
-  <si>
     <t>\pRatioInputInputFlow</t>
   </si>
   <si>
@@ -654,10 +624,127 @@
     <t>\Cdcg</t>
   </si>
   <si>
-    <t>Cdcg_{#1}</t>
-  </si>
-  <si>
     <t>Set of commodities of which the sum of the flows are restricted by the capacity of the unit</t>
+  </si>
+  <si>
+    <t>\pFlowBound</t>
+  </si>
+  <si>
+    <t>FlowBound</t>
+  </si>
+  <si>
+    <t>p^{FlowBound}_{#1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bound on (sum of) the absolute flows of commodities within commodity group cg entering or leaving unit u </t>
+  </si>
+  <si>
+    <t>ProductionShare</t>
+  </si>
+  <si>
+    <t>\pProductionShare</t>
+  </si>
+  <si>
+    <t>p^{ProductionShare}_{#1}</t>
+  </si>
+  <si>
+    <t>Bound on the share of the production of the commodities within commodity group cg entering or leaving unit u with respect to the total production of those commodities</t>
+  </si>
+  <si>
+    <t>ConsumptionShare</t>
+  </si>
+  <si>
+    <t>\pConsumptionShare</t>
+  </si>
+  <si>
+    <t>p^{ConsumptionShare}_{#1}</t>
+  </si>
+  <si>
+    <t>Bound on the share of the consumption of the commodities within commodity group cg entering or leaving unit u with respect to the total consumption of those commodities</t>
+  </si>
+  <si>
+    <t>\commodity,\node, \unit,in/out,\timestep</t>
+  </si>
+  <si>
+    <t>Nodes</t>
+  </si>
+  <si>
+    <t>\nodes</t>
+  </si>
+  <si>
+    <t>Set of nodes</t>
+  </si>
+  <si>
+    <t>\node</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Set of tuples of commodity and node</t>
+  </si>
+  <si>
+    <t>\node \in Nodes</t>
+  </si>
+  <si>
+    <t>CommoditiesNodes</t>
+  </si>
+  <si>
+    <t>\CommoditiesNodes</t>
+  </si>
+  <si>
+    <t>OutputCommoditiesUnits</t>
+  </si>
+  <si>
+    <t>\OutputCommoditiesUnits</t>
+  </si>
+  <si>
+    <t>Set of tuples of unit and output commodity</t>
+  </si>
+  <si>
+    <t>InputCommoditiesUnits</t>
+  </si>
+  <si>
+    <t>\InputCommoditiesUnits</t>
+  </si>
+  <si>
+    <t>Set of tuples of unit and input commodity</t>
+  </si>
+  <si>
+    <t>OutputCommoditiesUnitsNodes</t>
+  </si>
+  <si>
+    <t>InputCommoditiesUnitsNodes</t>
+  </si>
+  <si>
+    <t>\OutputCommoditiesUnitsNodes</t>
+  </si>
+  <si>
+    <t>\InputCommoditiesUnitsNodes</t>
+  </si>
+  <si>
+    <t>Set of tuples of unit, output commodity and node</t>
+  </si>
+  <si>
+    <t>Set of tuples of unit and input commodity and node</t>
+  </si>
+  <si>
+    <t>(\commodity, \node) \in CommoditiesNodes</t>
+  </si>
+  <si>
+    <t>(\commodity, \unit) \in Cdcg</t>
+  </si>
+  <si>
+    <t>(\commodity, \unit) \in OutputCommoditiesUnits</t>
+  </si>
+  <si>
+    <t>(\commodity, \unit) \in InputCommoditiesUnits</t>
+  </si>
+  <si>
+    <t>(\commodity, \unit, \node) \in OutputCommoditiesUnitsNodes</t>
+  </si>
+  <si>
+    <t>(\commodity, \unit, \node) \in InputCommoditiesUnitsNodes</t>
   </si>
 </sst>
 </file>
@@ -1203,8 +1290,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q260" totalsRowShown="0">
-  <autoFilter ref="A1:Q260"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q268" totalsRowShown="0">
+  <autoFilter ref="A1:Q268"/>
   <sortState ref="A2:O136">
     <sortCondition ref="D1:D136"/>
   </sortState>
@@ -1494,31 +1581,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q260"/>
+  <dimension ref="A1:Q268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="88" customWidth="1"/>
-    <col min="4" max="4" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.453125" customWidth="1"/>
-    <col min="13" max="13" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" customWidth="1"/>
+    <col min="13" max="13" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1553,7 +1640,7 @@
         <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M1" t="s">
         <v>24</v>
@@ -1571,7 +1658,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1594,7 +1681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1617,18 +1704,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>214</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>217</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>218</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1640,18 +1727,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>155</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1663,18 +1750,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>184</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>185</v>
+        <v>11</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1686,24 +1773,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>173</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>174</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1715,24 +1796,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1744,21 +1825,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>167</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>168</v>
+        <v>43</v>
       </c>
       <c r="I9" t="s">
         <v>32</v>
@@ -1773,21 +1854,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>214</v>
       </c>
       <c r="D10" t="s">
-        <v>170</v>
+        <v>215</v>
       </c>
       <c r="F10" t="s">
-        <v>172</v>
+        <v>220</v>
       </c>
       <c r="G10" t="s">
-        <v>171</v>
+        <v>216</v>
       </c>
       <c r="I10" t="s">
         <v>32</v>
@@ -1802,24 +1883,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>221</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>222</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>235</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>219</v>
       </c>
       <c r="I11" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1831,24 +1912,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="D12" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="F12" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="G12" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="I12" t="s">
-        <v>182</v>
+        <v>60</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -1860,27 +1941,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="D13" t="s">
-        <v>209</v>
-      </c>
-      <c r="E13" t="s">
-        <v>63</v>
+        <v>224</v>
       </c>
       <c r="F13" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
       <c r="G13" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="I13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1892,27 +1970,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" t="s">
-        <v>63</v>
+        <v>227</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>238</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>228</v>
       </c>
       <c r="I14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1924,27 +1999,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" t="s">
-        <v>63</v>
+        <v>231</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>239</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="I15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1956,27 +2028,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>174</v>
+        <v>230</v>
       </c>
       <c r="D16" t="s">
-        <v>175</v>
-      </c>
-      <c r="E16" t="s">
-        <v>189</v>
+        <v>232</v>
       </c>
       <c r="F16" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="G16" t="s">
-        <v>177</v>
+        <v>234</v>
       </c>
       <c r="I16" t="s">
-        <v>178</v>
+        <v>60</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1988,59 +2057,53 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D17" t="s">
-        <v>156</v>
-      </c>
-      <c r="E17" t="s">
-        <v>10</v>
+        <v>157</v>
       </c>
       <c r="F17" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="G17" t="s">
         <v>158</v>
       </c>
       <c r="I17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
         <v>159</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>101</v>
-      </c>
       <c r="D18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" t="s">
-        <v>67</v>
+        <v>160</v>
       </c>
       <c r="F18" t="s">
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
+        <v>161</v>
       </c>
       <c r="I18" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -2052,27 +2115,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="I19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -2084,27 +2144,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>169</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" t="s">
-        <v>49</v>
+        <v>170</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>191</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="I20" t="s">
-        <v>60</v>
+        <v>172</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -2116,27 +2173,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>165</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="F21" t="s">
-        <v>82</v>
+        <v>166</v>
       </c>
       <c r="G21" t="s">
-        <v>58</v>
+        <v>167</v>
       </c>
       <c r="I21" t="s">
-        <v>59</v>
+        <v>168</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -2148,27 +2205,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>146</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>92</v>
+        <v>147</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>148</v>
       </c>
       <c r="I22" t="s">
-        <v>59</v>
+        <v>149</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -2180,27 +2237,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="G23" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="I23" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2212,27 +2269,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>113</v>
+        <v>34</v>
       </c>
       <c r="F24" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G24" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="I24" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -2244,27 +2301,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D25" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F25" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="G25" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -2276,27 +2333,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="G26" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
       <c r="I26" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -2308,27 +2365,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="G27" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="I27" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -2340,27 +2397,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="E28" t="s">
-        <v>148</v>
+        <v>56</v>
       </c>
       <c r="F28" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="G28" t="s">
-        <v>140</v>
+        <v>85</v>
       </c>
       <c r="I28" t="s">
-        <v>141</v>
+        <v>58</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2372,27 +2429,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>202</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>201</v>
       </c>
       <c r="E29" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="F29" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="G29" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
       <c r="I29" t="s">
-        <v>141</v>
+        <v>58</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -2404,27 +2461,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>205</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="E30" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="F30" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="G30" t="s">
-        <v>154</v>
+        <v>208</v>
       </c>
       <c r="I30" t="s">
-        <v>141</v>
+        <v>58</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -2436,27 +2493,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>209</v>
       </c>
       <c r="D31" t="s">
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="E31" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="F31" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="G31" t="s">
-        <v>153</v>
+        <v>212</v>
       </c>
       <c r="I31" t="s">
-        <v>141</v>
+        <v>58</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -2468,27 +2525,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>203</v>
+        <v>102</v>
       </c>
       <c r="D32" t="s">
-        <v>202</v>
+        <v>98</v>
       </c>
       <c r="E32" t="s">
-        <v>204</v>
+        <v>103</v>
       </c>
       <c r="F32" t="s">
-        <v>205</v>
+        <v>99</v>
       </c>
       <c r="G32" t="s">
-        <v>206</v>
+        <v>100</v>
       </c>
       <c r="I32" t="s">
-        <v>207</v>
+        <v>101</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -2500,425 +2557,681 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
       <c r="C33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" t="s">
+        <v>106</v>
+      </c>
+      <c r="G33" t="s">
+        <v>107</v>
+      </c>
+      <c r="I33" t="s">
+        <v>101</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" t="s">
+        <v>117</v>
+      </c>
+      <c r="G34" t="s">
+        <v>118</v>
+      </c>
+      <c r="I34" t="s">
+        <v>101</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" t="s">
+        <v>120</v>
+      </c>
+      <c r="E35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" t="s">
+        <v>121</v>
+      </c>
+      <c r="G35" t="s">
+        <v>122</v>
+      </c>
+      <c r="I35" t="s">
+        <v>101</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" t="s">
+        <v>138</v>
+      </c>
+      <c r="F36" t="s">
+        <v>129</v>
+      </c>
+      <c r="G36" t="s">
+        <v>130</v>
+      </c>
+      <c r="I36" t="s">
+        <v>131</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" t="s">
+        <v>134</v>
+      </c>
+      <c r="G37" t="s">
+        <v>135</v>
+      </c>
+      <c r="I37" t="s">
+        <v>131</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" t="s">
+        <v>139</v>
+      </c>
+      <c r="G38" t="s">
+        <v>144</v>
+      </c>
+      <c r="I38" t="s">
+        <v>131</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" t="s">
+        <v>141</v>
+      </c>
+      <c r="E39" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" t="s">
+        <v>142</v>
+      </c>
+      <c r="G39" t="s">
+        <v>143</v>
+      </c>
+      <c r="I39" t="s">
+        <v>131</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>193</v>
+      </c>
+      <c r="D40" t="s">
+        <v>192</v>
+      </c>
+      <c r="E40" t="s">
+        <v>194</v>
+      </c>
+      <c r="F40" t="s">
+        <v>195</v>
+      </c>
+      <c r="G40" t="s">
+        <v>196</v>
+      </c>
+      <c r="I40" t="s">
+        <v>197</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>176</v>
+      </c>
+      <c r="D41" t="s">
+        <v>177</v>
+      </c>
+      <c r="E41" t="s">
+        <v>179</v>
+      </c>
+      <c r="F41" t="s">
+        <v>178</v>
+      </c>
+      <c r="G41" t="s">
+        <v>190</v>
+      </c>
+      <c r="I41" t="s">
+        <v>180</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
         <v>186</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D42" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" t="s">
+        <v>151</v>
+      </c>
+      <c r="G42" t="s">
+        <v>152</v>
+      </c>
+      <c r="I42" t="s">
+        <v>153</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
+        <v>213</v>
+      </c>
+      <c r="F43" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I43" t="s">
+        <v>78</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" t="s">
+        <v>112</v>
+      </c>
+      <c r="G44" t="s">
+        <v>188</v>
+      </c>
+      <c r="I44" t="s">
+        <v>114</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" t="s">
+        <v>49</v>
+      </c>
+      <c r="F45" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" t="s">
+        <v>189</v>
+      </c>
+      <c r="I45" t="s">
+        <v>114</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" t="s">
+        <v>49</v>
+      </c>
+      <c r="F46" t="s">
+        <v>96</v>
+      </c>
+      <c r="G46" t="s">
+        <v>97</v>
+      </c>
+      <c r="I46" t="s">
+        <v>114</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" t="s">
+        <v>124</v>
+      </c>
+      <c r="E47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" t="s">
+        <v>125</v>
+      </c>
+      <c r="G47" t="s">
+        <v>126</v>
+      </c>
+      <c r="I47" t="s">
+        <v>114</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" t="s">
+        <v>72</v>
+      </c>
+      <c r="G48" t="s">
+        <v>64</v>
+      </c>
+      <c r="I48" t="s">
+        <v>79</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>181</v>
+      </c>
+      <c r="D49" t="s">
+        <v>182</v>
+      </c>
+      <c r="E49" t="s">
+        <v>183</v>
+      </c>
+      <c r="F49" t="s">
+        <v>184</v>
+      </c>
+      <c r="G49" t="s">
         <v>187</v>
       </c>
-      <c r="E33" t="s">
-        <v>189</v>
-      </c>
-      <c r="F33" t="s">
-        <v>188</v>
-      </c>
-      <c r="G33" t="s">
-        <v>200</v>
-      </c>
-      <c r="I33" t="s">
-        <v>190</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>196</v>
-      </c>
-      <c r="D34" t="s">
-        <v>160</v>
-      </c>
-      <c r="E34" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" t="s">
-        <v>161</v>
-      </c>
-      <c r="G34" t="s">
-        <v>162</v>
-      </c>
-      <c r="I34" t="s">
-        <v>163</v>
-      </c>
-      <c r="J34">
-        <v>1</v>
-      </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" t="s">
-        <v>103</v>
-      </c>
-      <c r="D35" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" t="s">
-        <v>81</v>
-      </c>
-      <c r="G35" t="s">
-        <v>51</v>
-      </c>
-      <c r="I35" t="s">
-        <v>86</v>
-      </c>
-      <c r="J35">
-        <v>1</v>
-      </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
-      <c r="L35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" t="s">
-        <v>120</v>
-      </c>
-      <c r="E36" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" t="s">
-        <v>122</v>
-      </c>
-      <c r="G36" t="s">
-        <v>198</v>
-      </c>
-      <c r="I36" t="s">
-        <v>124</v>
-      </c>
-      <c r="J36">
-        <v>1</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>118</v>
-      </c>
-      <c r="D37" t="s">
-        <v>121</v>
-      </c>
-      <c r="E37" t="s">
-        <v>49</v>
-      </c>
-      <c r="F37" t="s">
-        <v>123</v>
-      </c>
-      <c r="G37" t="s">
-        <v>199</v>
-      </c>
-      <c r="I37" t="s">
-        <v>124</v>
-      </c>
-      <c r="J37">
-        <v>1</v>
-      </c>
-      <c r="K37">
-        <v>1</v>
-      </c>
-      <c r="L37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" t="s">
-        <v>105</v>
-      </c>
-      <c r="E38" t="s">
-        <v>49</v>
-      </c>
-      <c r="F38" t="s">
-        <v>106</v>
-      </c>
-      <c r="G38" t="s">
-        <v>107</v>
-      </c>
-      <c r="I38" t="s">
-        <v>124</v>
-      </c>
-      <c r="J38">
-        <v>1</v>
-      </c>
-      <c r="K38">
-        <v>1</v>
-      </c>
-      <c r="L38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" t="s">
-        <v>133</v>
-      </c>
-      <c r="D39" t="s">
-        <v>134</v>
-      </c>
-      <c r="E39" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" t="s">
-        <v>135</v>
-      </c>
-      <c r="G39" t="s">
-        <v>136</v>
-      </c>
-      <c r="I39" t="s">
-        <v>124</v>
-      </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-      <c r="K39">
-        <v>1</v>
-      </c>
-      <c r="L39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
-        <v>104</v>
-      </c>
-      <c r="D40" t="s">
-        <v>75</v>
-      </c>
-      <c r="E40" t="s">
-        <v>34</v>
-      </c>
-      <c r="F40" t="s">
-        <v>80</v>
-      </c>
-      <c r="G40" t="s">
-        <v>72</v>
-      </c>
-      <c r="I40" t="s">
-        <v>87</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
-      <c r="L40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" t="s">
-        <v>191</v>
-      </c>
-      <c r="D41" t="s">
-        <v>192</v>
-      </c>
-      <c r="E41" t="s">
-        <v>193</v>
-      </c>
-      <c r="F41" t="s">
-        <v>194</v>
-      </c>
-      <c r="G41" t="s">
-        <v>197</v>
-      </c>
-      <c r="I41" t="s">
-        <v>195</v>
-      </c>
-      <c r="J41">
-        <v>1</v>
-      </c>
-      <c r="K41">
-        <v>1</v>
-      </c>
-      <c r="L41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E103" s="1"/>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A239" t="s">
-        <v>14</v>
-      </c>
-      <c r="C239" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A240" t="s">
-        <v>8</v>
-      </c>
-      <c r="C240" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A241" t="s">
-        <v>8</v>
-      </c>
-      <c r="C241" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A242" t="s">
-        <v>8</v>
-      </c>
-      <c r="C242" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A243" t="s">
-        <v>6</v>
-      </c>
-      <c r="C243" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A244" t="s">
-        <v>7</v>
-      </c>
-      <c r="C244" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A245" t="s">
-        <v>6</v>
-      </c>
-      <c r="C245" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A246" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="I49" t="s">
+        <v>185</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E111" s="1"/>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C247" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="C248" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="C249" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="C250" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="C251" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="C252" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="C253" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added transmission equations To do: representation of el Net representation
</commit_message>
<xml_diff>
--- a/Model_formulation/00_nomenclature_definition.xlsx
+++ b/Model_formulation/00_nomenclature_definition.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="296">
   <si>
     <t>latexcommand</t>
   </si>
@@ -859,6 +859,57 @@
   </si>
   <si>
     <t>losses through transmission $n_i$ to $n_j$</t>
+  </si>
+  <si>
+    <t>\node_i,\node_j</t>
+  </si>
+  <si>
+    <t>\ptranstocap</t>
+  </si>
+  <si>
+    <t>p^{TransToCap}_{#1}</t>
+  </si>
+  <si>
+    <t>Conversion factor from transmitted flow to unit of capacity</t>
+  </si>
+  <si>
+    <t>Conversion Transmitted Flow to Capacity</t>
+  </si>
+  <si>
+    <t>\node,\timestep</t>
+  </si>
+  <si>
+    <t>\connection,\timestep</t>
+  </si>
+  <si>
+    <t>\nodesconnection</t>
+  </si>
+  <si>
+    <t>Set of nodes tuples and corresponding connection</t>
+  </si>
+  <si>
+    <t>Addigning node pairs to con</t>
+  </si>
+  <si>
+    <t>(\connection,\node_i,\node_j) \in NodepairConnection</t>
+  </si>
+  <si>
+    <t>\conalpha</t>
+  </si>
+  <si>
+    <t>Assigning flows to binary</t>
+  </si>
+  <si>
+    <t>\conbeta</t>
+  </si>
+  <si>
+    <t>Set of nodes and corresponding binary</t>
+  </si>
+  <si>
+    <t>(\node_i,\node_j,\al)</t>
+  </si>
+  <si>
+    <t>(\node_i,\node_j,\be)</t>
   </si>
 </sst>
 </file>
@@ -1404,8 +1455,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q271" totalsRowShown="0">
-  <autoFilter ref="A1:Q271"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q275" totalsRowShown="0">
+  <autoFilter ref="A1:Q275"/>
   <sortState ref="A2:O136">
     <sortCondition ref="D1:D136"/>
   </sortState>
@@ -1695,11 +1746,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q271"/>
+  <dimension ref="A1:Q275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M45" sqref="M45"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,25 +2424,22 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>288</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
+        <v>286</v>
       </c>
       <c r="F24" t="s">
-        <v>147</v>
+        <v>289</v>
       </c>
       <c r="G24" t="s">
-        <v>148</v>
+        <v>287</v>
       </c>
       <c r="I24" t="s">
-        <v>149</v>
+        <v>60</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -2405,25 +2453,22 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>291</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" t="s">
-        <v>61</v>
+        <v>290</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>294</v>
       </c>
       <c r="G25" t="s">
-        <v>62</v>
+        <v>293</v>
       </c>
       <c r="I25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -2437,25 +2482,22 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>291</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" t="s">
-        <v>34</v>
+        <v>292</v>
       </c>
       <c r="F26" t="s">
-        <v>77</v>
+        <v>295</v>
       </c>
       <c r="G26" t="s">
-        <v>65</v>
+        <v>293</v>
       </c>
       <c r="I26" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -2472,22 +2514,22 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>146</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>75</v>
+        <v>147</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>148</v>
       </c>
       <c r="I27" t="s">
-        <v>59</v>
+        <v>149</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -2504,22 +2546,22 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>284</v>
       </c>
       <c r="F28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G28" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I28" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2536,22 +2578,22 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="F29" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G29" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="I29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -2568,22 +2610,22 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G30" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="I30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -2600,19 +2642,19 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>202</v>
+        <v>87</v>
       </c>
       <c r="D31" t="s">
-        <v>201</v>
+        <v>71</v>
       </c>
       <c r="E31" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="F31" t="s">
-        <v>203</v>
+        <v>74</v>
       </c>
       <c r="G31" t="s">
-        <v>204</v>
+        <v>57</v>
       </c>
       <c r="I31" t="s">
         <v>58</v>
@@ -2632,19 +2674,19 @@
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>205</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>206</v>
+        <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="F32" t="s">
-        <v>207</v>
+        <v>82</v>
       </c>
       <c r="G32" t="s">
-        <v>208</v>
+        <v>84</v>
       </c>
       <c r="I32" t="s">
         <v>58</v>
@@ -2664,19 +2706,19 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>209</v>
+        <v>89</v>
       </c>
       <c r="D33" t="s">
-        <v>210</v>
+        <v>81</v>
       </c>
       <c r="E33" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="F33" t="s">
-        <v>211</v>
+        <v>83</v>
       </c>
       <c r="G33" t="s">
-        <v>212</v>
+        <v>85</v>
       </c>
       <c r="I33" t="s">
         <v>58</v>
@@ -2696,22 +2738,22 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>202</v>
       </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>201</v>
       </c>
       <c r="E34" t="s">
         <v>103</v>
       </c>
       <c r="F34" t="s">
-        <v>99</v>
+        <v>203</v>
       </c>
       <c r="G34" t="s">
-        <v>100</v>
+        <v>204</v>
       </c>
       <c r="I34" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -2728,22 +2770,22 @@
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="D35" t="s">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="E35" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="F35" t="s">
-        <v>106</v>
+        <v>207</v>
       </c>
       <c r="G35" t="s">
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="I35" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -2760,22 +2802,22 @@
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>209</v>
       </c>
       <c r="D36" t="s">
-        <v>116</v>
+        <v>210</v>
       </c>
       <c r="E36" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="F36" t="s">
-        <v>117</v>
+        <v>211</v>
       </c>
       <c r="G36" t="s">
-        <v>118</v>
+        <v>212</v>
       </c>
       <c r="I36" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -2792,19 +2834,19 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="D37" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="E37" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="F37" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="G37" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="I37" t="s">
         <v>101</v>
@@ -2824,22 +2866,22 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="E38" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="F38" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="G38" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="I38" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -2856,22 +2898,22 @@
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D39" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="F39" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="G39" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="I39" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="J39">
         <v>1</v>
@@ -2888,22 +2930,22 @@
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D40" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="F40" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="G40" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="I40" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="J40">
         <v>1</v>
@@ -2920,19 +2962,19 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E41" t="s">
         <v>138</v>
       </c>
       <c r="F41" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="G41" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="I41" t="s">
         <v>131</v>
@@ -2952,22 +2994,22 @@
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>193</v>
+        <v>132</v>
       </c>
       <c r="D42" t="s">
-        <v>192</v>
+        <v>133</v>
       </c>
       <c r="E42" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="F42" t="s">
-        <v>195</v>
+        <v>134</v>
       </c>
       <c r="G42" t="s">
-        <v>196</v>
+        <v>135</v>
       </c>
       <c r="I42" t="s">
-        <v>197</v>
+        <v>131</v>
       </c>
       <c r="J42">
         <v>1</v>
@@ -2984,22 +3026,22 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="D43" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
       <c r="E43" t="s">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="F43" t="s">
-        <v>178</v>
+        <v>139</v>
       </c>
       <c r="G43" t="s">
-        <v>190</v>
+        <v>144</v>
       </c>
       <c r="I43" t="s">
-        <v>180</v>
+        <v>131</v>
       </c>
       <c r="J43">
         <v>1</v>
@@ -3016,22 +3058,22 @@
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>257</v>
+        <v>140</v>
       </c>
       <c r="D44" t="s">
-        <v>258</v>
+        <v>141</v>
       </c>
       <c r="E44" t="s">
-        <v>243</v>
+        <v>138</v>
       </c>
       <c r="F44" t="s">
-        <v>259</v>
+        <v>142</v>
       </c>
       <c r="G44" t="s">
-        <v>260</v>
+        <v>143</v>
       </c>
       <c r="I44" t="s">
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="J44">
         <v>1</v>
@@ -3048,22 +3090,22 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>274</v>
+        <v>193</v>
       </c>
       <c r="D45" t="s">
-        <v>275</v>
+        <v>192</v>
       </c>
       <c r="E45" t="s">
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="F45" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="G45" t="s">
-        <v>278</v>
+        <v>196</v>
       </c>
       <c r="I45" t="s">
-        <v>60</v>
+        <v>197</v>
       </c>
       <c r="J45">
         <v>1</v>
@@ -3077,25 +3119,25 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>186</v>
+        <v>283</v>
       </c>
       <c r="D46" t="s">
-        <v>150</v>
+        <v>280</v>
       </c>
       <c r="E46" t="s">
-        <v>61</v>
+        <v>279</v>
       </c>
       <c r="F46" t="s">
-        <v>151</v>
+        <v>281</v>
       </c>
       <c r="G46" t="s">
-        <v>152</v>
+        <v>282</v>
       </c>
       <c r="I46" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="J46">
         <v>1</v>
@@ -3109,25 +3151,25 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>176</v>
       </c>
       <c r="D47" t="s">
-        <v>66</v>
+        <v>177</v>
       </c>
       <c r="E47" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
       <c r="F47" t="s">
-        <v>73</v>
+        <v>178</v>
       </c>
       <c r="G47" t="s">
-        <v>50</v>
+        <v>190</v>
       </c>
       <c r="I47" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
       <c r="J47">
         <v>1</v>
@@ -3141,25 +3183,25 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>86</v>
+        <v>257</v>
       </c>
       <c r="D48" t="s">
-        <v>110</v>
+        <v>258</v>
       </c>
       <c r="E48" t="s">
-        <v>49</v>
+        <v>276</v>
       </c>
       <c r="F48" t="s">
-        <v>112</v>
+        <v>259</v>
       </c>
       <c r="G48" t="s">
-        <v>188</v>
+        <v>260</v>
       </c>
       <c r="I48" t="s">
-        <v>114</v>
+        <v>60</v>
       </c>
       <c r="J48">
         <v>1</v>
@@ -3173,25 +3215,25 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>108</v>
+        <v>274</v>
       </c>
       <c r="D49" t="s">
-        <v>111</v>
+        <v>275</v>
       </c>
       <c r="E49" t="s">
-        <v>49</v>
+        <v>279</v>
       </c>
       <c r="F49" t="s">
-        <v>113</v>
+        <v>277</v>
       </c>
       <c r="G49" t="s">
-        <v>189</v>
+        <v>278</v>
       </c>
       <c r="I49" t="s">
-        <v>114</v>
+        <v>60</v>
       </c>
       <c r="J49">
         <v>1</v>
@@ -3208,22 +3250,22 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
+        <v>186</v>
       </c>
       <c r="D50" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="E50" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F50" t="s">
-        <v>96</v>
+        <v>151</v>
       </c>
       <c r="G50" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="I50" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="J50">
         <v>1</v>
@@ -3240,22 +3282,22 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D51" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="E51" t="s">
-        <v>49</v>
+        <v>213</v>
       </c>
       <c r="F51" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="G51" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="I51" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="J51">
         <v>1</v>
@@ -3272,22 +3314,22 @@
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D52" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="E52" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F52" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="G52" t="s">
-        <v>64</v>
+        <v>188</v>
       </c>
       <c r="I52" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="J52">
         <v>1</v>
@@ -3304,22 +3346,22 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>181</v>
+        <v>108</v>
       </c>
       <c r="D53" t="s">
-        <v>182</v>
+        <v>111</v>
       </c>
       <c r="E53" t="s">
-        <v>183</v>
+        <v>49</v>
       </c>
       <c r="F53" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
       <c r="G53" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I53" t="s">
-        <v>185</v>
+        <v>114</v>
       </c>
       <c r="J53">
         <v>1</v>
@@ -3336,22 +3378,22 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>246</v>
+        <v>109</v>
       </c>
       <c r="D54" t="s">
-        <v>247</v>
+        <v>95</v>
       </c>
       <c r="E54" t="s">
-        <v>251</v>
+        <v>49</v>
       </c>
       <c r="F54" t="s">
-        <v>248</v>
+        <v>96</v>
       </c>
       <c r="G54" t="s">
-        <v>256</v>
+        <v>97</v>
       </c>
       <c r="I54" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="J54">
         <v>1</v>
@@ -3368,22 +3410,22 @@
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>252</v>
+        <v>123</v>
       </c>
       <c r="D55" t="s">
-        <v>253</v>
+        <v>124</v>
       </c>
       <c r="E55" t="s">
-        <v>251</v>
+        <v>49</v>
       </c>
       <c r="F55" t="s">
-        <v>254</v>
+        <v>125</v>
       </c>
       <c r="G55" t="s">
-        <v>255</v>
+        <v>126</v>
       </c>
       <c r="I55" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="J55">
         <v>1</v>
@@ -3400,22 +3442,22 @@
         <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>261</v>
+        <v>94</v>
       </c>
       <c r="D56" t="s">
-        <v>270</v>
+        <v>67</v>
       </c>
       <c r="E56" t="s">
-        <v>251</v>
+        <v>34</v>
       </c>
       <c r="F56" t="s">
-        <v>265</v>
+        <v>72</v>
       </c>
       <c r="G56" t="s">
-        <v>269</v>
+        <v>64</v>
       </c>
       <c r="I56" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="J56">
         <v>1</v>
@@ -3432,22 +3474,22 @@
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>262</v>
+        <v>181</v>
       </c>
       <c r="D57" t="s">
-        <v>271</v>
+        <v>182</v>
       </c>
       <c r="E57" t="s">
-        <v>251</v>
+        <v>183</v>
       </c>
       <c r="F57" t="s">
-        <v>266</v>
+        <v>184</v>
       </c>
       <c r="G57" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="I57" t="s">
-        <v>60</v>
+        <v>185</v>
       </c>
       <c r="J57">
         <v>1</v>
@@ -3464,19 +3506,19 @@
         <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="D58" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="E58" t="s">
         <v>251</v>
       </c>
       <c r="F58" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="G58" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="I58" t="s">
         <v>60</v>
@@ -3496,19 +3538,19 @@
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="D59" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="E59" t="s">
         <v>251</v>
       </c>
       <c r="F59" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="G59" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="I59" t="s">
         <v>60</v>
@@ -3523,137 +3565,265 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E114" s="1"/>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>14</v>
-      </c>
-      <c r="C250" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>8</v>
-      </c>
-      <c r="C251" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>8</v>
-      </c>
-      <c r="C252" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>8</v>
-      </c>
-      <c r="C253" t="s">
-        <v>9</v>
-      </c>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>261</v>
+      </c>
+      <c r="D60" t="s">
+        <v>270</v>
+      </c>
+      <c r="E60" t="s">
+        <v>285</v>
+      </c>
+      <c r="F60" t="s">
+        <v>265</v>
+      </c>
+      <c r="G60" t="s">
+        <v>269</v>
+      </c>
+      <c r="I60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>262</v>
+      </c>
+      <c r="D61" t="s">
+        <v>271</v>
+      </c>
+      <c r="E61" t="s">
+        <v>285</v>
+      </c>
+      <c r="F61" t="s">
+        <v>266</v>
+      </c>
+      <c r="G61" t="s">
+        <v>269</v>
+      </c>
+      <c r="I61" t="s">
+        <v>60</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>263</v>
+      </c>
+      <c r="D62" t="s">
+        <v>272</v>
+      </c>
+      <c r="E62" t="s">
+        <v>251</v>
+      </c>
+      <c r="F62" t="s">
+        <v>268</v>
+      </c>
+      <c r="G62" t="s">
+        <v>269</v>
+      </c>
+      <c r="I62" t="s">
+        <v>60</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>264</v>
+      </c>
+      <c r="D63" t="s">
+        <v>273</v>
+      </c>
+      <c r="E63" t="s">
+        <v>251</v>
+      </c>
+      <c r="F63" t="s">
+        <v>267</v>
+      </c>
+      <c r="G63" t="s">
+        <v>269</v>
+      </c>
+      <c r="I63" t="s">
+        <v>60</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="1"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C254" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C255" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
+        <v>8</v>
+      </c>
+      <c r="C256" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>8</v>
+      </c>
+      <c r="C257" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
         <v>6</v>
       </c>
-      <c r="C256" t="s">
+      <c r="C258" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C259" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C260" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel merge, julia delete
</commit_message>
<xml_diff>
--- a/Model_formulation/00_nomenclature_definition.xlsx
+++ b/Model_formulation/00_nomenclature_definition.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0093836\Box Sync\My Webspace\Post-doc\Spine\WP3\model\Model_formulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0122387\Documents\Spine project\model\Model_formulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="17970" windowHeight="5930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10155" windowHeight="1950"/>
   </bookViews>
   <sheets>
     <sheet name="00_nomenclature_definition" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="440">
   <si>
     <t>latexcommand</t>
   </si>
@@ -1177,6 +1177,171 @@
   </si>
   <si>
     <t>Number of Units</t>
+  </si>
+  <si>
+    <t>Connections</t>
+  </si>
+  <si>
+    <t>\connections</t>
+  </si>
+  <si>
+    <t>\connection \in Connections</t>
+  </si>
+  <si>
+    <t>Set of connections</t>
+  </si>
+  <si>
+    <t>Addigning node pairs to con</t>
+  </si>
+  <si>
+    <t>\nodesconnection</t>
+  </si>
+  <si>
+    <t>(\connection,\node_i,\node_j) \in NodepairConnection</t>
+  </si>
+  <si>
+    <t>Set of nodes tuples and corresponding connection</t>
+  </si>
+  <si>
+    <t>Assigning flows to binary</t>
+  </si>
+  <si>
+    <t>\conalpha</t>
+  </si>
+  <si>
+    <t>(\node_i,\node_j,\al)</t>
+  </si>
+  <si>
+    <t>Set of nodes and corresponding binary</t>
+  </si>
+  <si>
+    <t>\conbeta</t>
+  </si>
+  <si>
+    <t>(\node_i,\node_j,\be)</t>
+  </si>
+  <si>
+    <t>\node,\timestep</t>
+  </si>
+  <si>
+    <t>Conversion Transmitted Flow to Capacity</t>
+  </si>
+  <si>
+    <t>\ptranstocap</t>
+  </si>
+  <si>
+    <t>\node_i,\node_j</t>
+  </si>
+  <si>
+    <t>p^{TransToCap}_{#1}</t>
+  </si>
+  <si>
+    <t>Conversion factor from transmitted flow to unit of capacity</t>
+  </si>
+  <si>
+    <t>max. TransCapa</t>
+  </si>
+  <si>
+    <t>\pMaxTransCapa</t>
+  </si>
+  <si>
+    <t>\connection,\node_i,\node_j</t>
+  </si>
+  <si>
+    <t>p^{max.TransCapa}_{#1}</t>
+  </si>
+  <si>
+    <t>max. possible transmission Capacity</t>
+  </si>
+  <si>
+    <t>Transmission losses</t>
+  </si>
+  <si>
+    <t>\ptransloss</t>
+  </si>
+  <si>
+    <t>p^{loss}_{#1}</t>
+  </si>
+  <si>
+    <t>losses through transmission $n_i$ to $n_j$</t>
+  </si>
+  <si>
+    <t>\vTrans</t>
+  </si>
+  <si>
+    <t>\connection,\node_i,\node_j,\timestep</t>
+  </si>
+  <si>
+    <t>v^{Trans}_{#1}</t>
+  </si>
+  <si>
+    <t>Import by $n_i$ from $n_j$</t>
+  </si>
+  <si>
+    <t>\vTranCapa</t>
+  </si>
+  <si>
+    <t>v^{TransCapa}_{#1}</t>
+  </si>
+  <si>
+    <t>Capacity from $n_j$ to $n_i$</t>
+  </si>
+  <si>
+    <t>\al</t>
+  </si>
+  <si>
+    <t>\connection,\timestep</t>
+  </si>
+  <si>
+    <t>\alpha^{Trans}_{#1}</t>
+  </si>
+  <si>
+    <t>decision</t>
+  </si>
+  <si>
+    <t>\be</t>
+  </si>
+  <si>
+    <t>\beta^{Trans}_{#1}</t>
+  </si>
+  <si>
+    <t>\ga</t>
+  </si>
+  <si>
+    <t>\gamma^{Trans}_{#1}</t>
+  </si>
+  <si>
+    <t>\de</t>
+  </si>
+  <si>
+    <t>\delta^{Trans}_{#1}</t>
+  </si>
+  <si>
+    <t>Transmission</t>
+  </si>
+  <si>
+    <t>TransCapa</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Connection</t>
+  </si>
+  <si>
+    <t>\connection</t>
+  </si>
+  <si>
+    <t>{con}</t>
   </si>
 </sst>
 </file>
@@ -1722,8 +1887,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q306" totalsRowShown="0">
-  <autoFilter ref="A1:Q306"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q314" totalsRowShown="0">
+  <autoFilter ref="A1:Q314"/>
   <sortState ref="A2:O136">
     <sortCondition ref="D1:D136"/>
   </sortState>
@@ -2013,31 +2178,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q306"/>
+  <dimension ref="A1:Q314"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="88" customWidth="1"/>
-    <col min="4" max="4" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.453125" customWidth="1"/>
-    <col min="13" max="13" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" customWidth="1"/>
+    <col min="13" max="13" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2090,7 +2255,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2113,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2136,7 +2301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2159,7 +2324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2182,18 +2347,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>437</v>
       </c>
       <c r="D6" t="s">
-        <v>186</v>
+        <v>438</v>
       </c>
       <c r="F6" t="s">
-        <v>187</v>
+        <v>439</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -2205,18 +2370,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
       <c r="F7" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -2228,18 +2393,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>220</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>221</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -2251,18 +2416,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>135</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -2274,48 +2439,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
         <v>154</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>155</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>156</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" t="s">
-        <v>52</v>
-      </c>
       <c r="J11">
         <v>1</v>
       </c>
@@ -2326,21 +2485,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>229</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>226</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>227</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s">
-        <v>228</v>
+        <v>38</v>
       </c>
       <c r="I12" t="s">
         <v>52</v>
@@ -2355,24 +2514,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>229</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>226</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>227</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>228</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -2384,21 +2543,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>230</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>231</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>232</v>
+        <v>46</v>
       </c>
       <c r="G14" t="s">
-        <v>233</v>
+        <v>43</v>
       </c>
       <c r="I14" t="s">
         <v>32</v>
@@ -2413,21 +2572,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c r="D15" t="s">
-        <v>184</v>
+        <v>231</v>
       </c>
       <c r="F15" t="s">
-        <v>189</v>
+        <v>232</v>
       </c>
       <c r="G15" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
       <c r="I15" t="s">
         <v>32</v>
@@ -2442,21 +2601,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>234</v>
+        <v>183</v>
       </c>
       <c r="D16" t="s">
-        <v>235</v>
+        <v>184</v>
       </c>
       <c r="F16" t="s">
-        <v>236</v>
+        <v>189</v>
       </c>
       <c r="G16" t="s">
-        <v>237</v>
+        <v>185</v>
       </c>
       <c r="I16" t="s">
         <v>32</v>
@@ -2471,21 +2630,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
       <c r="D17" t="s">
-        <v>191</v>
+        <v>235</v>
       </c>
       <c r="F17" t="s">
-        <v>204</v>
+        <v>236</v>
       </c>
       <c r="G17" t="s">
-        <v>188</v>
+        <v>237</v>
       </c>
       <c r="I17" t="s">
         <v>32</v>
@@ -2500,24 +2659,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="D18" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="F18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G18" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="I18" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -2529,21 +2688,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="D19" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="F19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G19" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="I19" t="s">
         <v>58</v>
@@ -2558,21 +2717,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D20" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G20" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I20" t="s">
         <v>58</v>
@@ -2587,21 +2746,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D21" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G21" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="I21" t="s">
         <v>58</v>
@@ -2616,21 +2775,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I22" t="s">
         <v>58</v>
@@ -2645,24 +2804,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="D23" t="s">
-        <v>138</v>
+        <v>201</v>
       </c>
       <c r="F23" t="s">
-        <v>144</v>
+        <v>209</v>
       </c>
       <c r="G23" t="s">
-        <v>139</v>
+        <v>203</v>
       </c>
       <c r="I23" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2674,24 +2833,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>140</v>
+        <v>385</v>
       </c>
       <c r="D24" t="s">
-        <v>141</v>
+        <v>386</v>
       </c>
       <c r="F24" t="s">
-        <v>143</v>
+        <v>387</v>
       </c>
       <c r="G24" t="s">
-        <v>142</v>
+        <v>388</v>
       </c>
       <c r="I24" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -2703,24 +2862,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>389</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>390</v>
       </c>
       <c r="F25" t="s">
-        <v>55</v>
+        <v>391</v>
       </c>
       <c r="G25" t="s">
-        <v>47</v>
+        <v>392</v>
       </c>
       <c r="I25" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -2732,24 +2891,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>150</v>
+        <v>393</v>
       </c>
       <c r="D26" t="s">
-        <v>151</v>
+        <v>394</v>
       </c>
       <c r="F26" t="s">
-        <v>172</v>
+        <v>395</v>
       </c>
       <c r="G26" t="s">
-        <v>152</v>
+        <v>396</v>
       </c>
       <c r="I26" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -2761,376 +2920,361 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
       <c r="C27" t="s">
+        <v>393</v>
+      </c>
+      <c r="D27" t="s">
+        <v>397</v>
+      </c>
+      <c r="F27" t="s">
+        <v>398</v>
+      </c>
+      <c r="G27" t="s">
+        <v>396</v>
+      </c>
+      <c r="I27" t="s">
+        <v>58</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" t="s">
+        <v>139</v>
+      </c>
+      <c r="I28" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" t="s">
+        <v>143</v>
+      </c>
+      <c r="G29" t="s">
+        <v>142</v>
+      </c>
+      <c r="I29" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" t="s">
+        <v>47</v>
+      </c>
+      <c r="I30" t="s">
+        <v>53</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D31" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" t="s">
+        <v>172</v>
+      </c>
+      <c r="G31" t="s">
+        <v>152</v>
+      </c>
+      <c r="I31" t="s">
+        <v>153</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
         <v>145</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D32" t="s">
         <v>146</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E32" t="s">
         <v>160</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F32" t="s">
         <v>147</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G32" t="s">
         <v>148</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I32" t="s">
         <v>149</v>
       </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
         <v>126</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D33" t="s">
         <v>127</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E33" t="s">
         <v>10</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F33" t="s">
         <v>128</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G33" t="s">
         <v>129</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I33" t="s">
         <v>130</v>
       </c>
-      <c r="J28">
-        <v>1</v>
-      </c>
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
         <v>75</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D34" t="s">
         <v>64</v>
       </c>
-      <c r="E29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="E34" t="s">
+        <v>399</v>
+      </c>
+      <c r="F34" t="s">
         <v>69</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G34" t="s">
         <v>60</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I34" t="s">
         <v>61</v>
       </c>
-      <c r="J29">
-        <v>1</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
         <v>378</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D35" t="s">
         <v>382</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E35" t="s">
         <v>34</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F35" t="s">
         <v>383</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G35" t="s">
         <v>384</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I35" t="s">
         <v>54</v>
       </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
         <v>74</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D36" t="s">
         <v>65</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E36" t="s">
         <v>34</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F36" t="s">
         <v>70</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G36" t="s">
         <v>62</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I36" t="s">
         <v>54</v>
       </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
         <v>76</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D37" t="s">
         <v>66</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E37" t="s">
         <v>49</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F37" t="s">
         <v>68</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G37" t="s">
         <v>26</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I37" t="s">
         <v>57</v>
       </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
-      <c r="L32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
         <v>238</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D38" t="s">
         <v>239</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E38" t="s">
         <v>210</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F38" t="s">
         <v>240</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G38" t="s">
         <v>241</v>
-      </c>
-      <c r="I33" t="s">
-        <v>56</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" t="s">
-        <v>242</v>
-      </c>
-      <c r="D34" t="s">
-        <v>243</v>
-      </c>
-      <c r="E34" t="s">
-        <v>210</v>
-      </c>
-      <c r="F34" t="s">
-        <v>244</v>
-      </c>
-      <c r="G34" t="s">
-        <v>245</v>
-      </c>
-      <c r="I34" t="s">
-        <v>56</v>
-      </c>
-      <c r="J34">
-        <v>1</v>
-      </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" t="s">
-        <v>246</v>
-      </c>
-      <c r="D35" t="s">
-        <v>265</v>
-      </c>
-      <c r="E35" t="s">
-        <v>210</v>
-      </c>
-      <c r="F35" t="s">
-        <v>247</v>
-      </c>
-      <c r="G35" t="s">
-        <v>248</v>
-      </c>
-      <c r="I35" t="s">
-        <v>56</v>
-      </c>
-      <c r="J35">
-        <v>1</v>
-      </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
-      <c r="L35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" t="s">
-        <v>249</v>
-      </c>
-      <c r="D36" t="s">
-        <v>251</v>
-      </c>
-      <c r="E36" t="s">
-        <v>211</v>
-      </c>
-      <c r="F36" t="s">
-        <v>253</v>
-      </c>
-      <c r="G36" t="s">
-        <v>255</v>
-      </c>
-      <c r="I36" t="s">
-        <v>56</v>
-      </c>
-      <c r="J36">
-        <v>1</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" t="s">
-        <v>250</v>
-      </c>
-      <c r="D37" t="s">
-        <v>252</v>
-      </c>
-      <c r="E37" t="s">
-        <v>211</v>
-      </c>
-      <c r="F37" t="s">
-        <v>254</v>
-      </c>
-      <c r="G37" t="s">
-        <v>256</v>
-      </c>
-      <c r="I37" t="s">
-        <v>56</v>
-      </c>
-      <c r="J37">
-        <v>1</v>
-      </c>
-      <c r="K37">
-        <v>1</v>
-      </c>
-      <c r="L37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" t="s">
-        <v>257</v>
-      </c>
-      <c r="D38" t="s">
-        <v>259</v>
-      </c>
-      <c r="E38" t="s">
-        <v>211</v>
-      </c>
-      <c r="F38" t="s">
-        <v>261</v>
-      </c>
-      <c r="G38" t="s">
-        <v>263</v>
       </c>
       <c r="I38" t="s">
         <v>56</v>
@@ -3145,24 +3289,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="D39" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="E39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F39" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="G39" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="I39" t="s">
         <v>56</v>
@@ -3177,24 +3321,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="D40" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E40" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="F40" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="G40" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
       <c r="I40" t="s">
         <v>56</v>
@@ -3209,24 +3353,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="D41" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="E41" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F41" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="G41" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="I41" t="s">
         <v>56</v>
@@ -3241,24 +3385,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="D42" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="E42" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F42" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="G42" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="I42" t="s">
         <v>56</v>
@@ -3273,24 +3417,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="D43" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
       <c r="E43" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F43" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="G43" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="I43" t="s">
         <v>56</v>
@@ -3305,24 +3449,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="D44" t="s">
-        <v>282</v>
+        <v>260</v>
       </c>
       <c r="E44" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F44" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="G44" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="I44" t="s">
         <v>56</v>
@@ -3337,24 +3481,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="D45" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="E45" t="s">
         <v>224</v>
       </c>
       <c r="F45" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="G45" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="I45" t="s">
         <v>56</v>
@@ -3369,24 +3513,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="D46" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="E46" t="s">
         <v>224</v>
       </c>
       <c r="F46" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="G46" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="I46" t="s">
         <v>56</v>
@@ -3401,24 +3545,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>297</v>
+        <v>268</v>
       </c>
       <c r="D47" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
       <c r="E47" t="s">
         <v>224</v>
       </c>
       <c r="F47" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="G47" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="I47" t="s">
         <v>56</v>
@@ -3433,24 +3577,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="D48" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="E48" t="s">
         <v>224</v>
       </c>
       <c r="F48" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="G48" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="I48" t="s">
         <v>56</v>
@@ -3465,24 +3609,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="D49" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="E49" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F49" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="G49" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="I49" t="s">
         <v>56</v>
@@ -3497,24 +3641,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="D50" t="s">
-        <v>313</v>
+        <v>283</v>
       </c>
       <c r="E50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F50" t="s">
-        <v>314</v>
+        <v>286</v>
       </c>
       <c r="G50" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="I50" t="s">
         <v>56</v>
@@ -3529,24 +3673,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>321</v>
+        <v>290</v>
       </c>
       <c r="D51" t="s">
-        <v>324</v>
+        <v>291</v>
       </c>
       <c r="E51" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F51" t="s">
-        <v>327</v>
+        <v>292</v>
       </c>
       <c r="G51" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="I51" t="s">
         <v>56</v>
@@ -3561,24 +3705,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="D52" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="E52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F52" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="G52" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="I52" t="s">
         <v>56</v>
@@ -3593,24 +3737,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="D53" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="E53" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F53" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="G53" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="I53" t="s">
         <v>56</v>
@@ -3625,24 +3769,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="D54" t="s">
-        <v>325</v>
+        <v>303</v>
       </c>
       <c r="E54" t="s">
         <v>225</v>
       </c>
       <c r="F54" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="G54" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
       <c r="I54" t="s">
         <v>56</v>
@@ -3657,24 +3801,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D55" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="E55" t="s">
         <v>225</v>
       </c>
       <c r="F55" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="G55" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="I55" t="s">
         <v>56</v>
@@ -3689,24 +3833,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D56" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="E56" t="s">
         <v>225</v>
       </c>
       <c r="F56" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="G56" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="I56" t="s">
         <v>56</v>
@@ -3721,24 +3865,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="D57" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="E57" t="s">
         <v>225</v>
       </c>
       <c r="F57" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="G57" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="I57" t="s">
         <v>56</v>
@@ -3753,24 +3897,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="D58" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="E58" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F58" t="s">
-        <v>338</v>
+        <v>315</v>
       </c>
       <c r="G58" t="s">
-        <v>342</v>
+        <v>288</v>
       </c>
       <c r="I58" t="s">
         <v>56</v>
@@ -3785,24 +3929,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="D59" t="s">
-        <v>350</v>
+        <v>325</v>
       </c>
       <c r="E59" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F59" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="G59" t="s">
-        <v>358</v>
+        <v>289</v>
       </c>
       <c r="I59" t="s">
         <v>56</v>
@@ -3817,24 +3961,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>362</v>
+        <v>311</v>
       </c>
       <c r="D60" t="s">
-        <v>369</v>
+        <v>309</v>
       </c>
       <c r="E60" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F60" t="s">
-        <v>370</v>
+        <v>307</v>
       </c>
       <c r="G60" t="s">
-        <v>374</v>
+        <v>293</v>
       </c>
       <c r="I60" t="s">
         <v>56</v>
@@ -3849,24 +3993,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="D61" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="E61" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F61" t="s">
-        <v>339</v>
+        <v>316</v>
       </c>
       <c r="G61" t="s">
-        <v>343</v>
+        <v>294</v>
       </c>
       <c r="I61" t="s">
         <v>56</v>
@@ -3881,24 +4025,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="D62" t="s">
-        <v>351</v>
+        <v>326</v>
       </c>
       <c r="E62" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F62" t="s">
-        <v>354</v>
+        <v>329</v>
       </c>
       <c r="G62" t="s">
-        <v>359</v>
+        <v>301</v>
       </c>
       <c r="I62" t="s">
         <v>56</v>
@@ -3913,24 +4057,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>363</v>
+        <v>330</v>
       </c>
       <c r="D63" t="s">
-        <v>366</v>
+        <v>334</v>
       </c>
       <c r="E63" t="s">
         <v>224</v>
       </c>
       <c r="F63" t="s">
-        <v>371</v>
+        <v>338</v>
       </c>
       <c r="G63" t="s">
-        <v>375</v>
+        <v>342</v>
       </c>
       <c r="I63" t="s">
         <v>56</v>
@@ -3945,24 +4089,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="D64" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="E64" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F64" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="G64" t="s">
-        <v>344</v>
+        <v>358</v>
       </c>
       <c r="I64" t="s">
         <v>56</v>
@@ -3977,24 +4121,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="D65" t="s">
-        <v>352</v>
+        <v>369</v>
       </c>
       <c r="E65" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F65" t="s">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="G65" t="s">
-        <v>360</v>
+        <v>374</v>
       </c>
       <c r="I65" t="s">
         <v>56</v>
@@ -4009,24 +4153,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>364</v>
+        <v>331</v>
       </c>
       <c r="D66" t="s">
-        <v>367</v>
+        <v>335</v>
       </c>
       <c r="E66" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F66" t="s">
-        <v>372</v>
+        <v>339</v>
       </c>
       <c r="G66" t="s">
-        <v>376</v>
+        <v>343</v>
       </c>
       <c r="I66" t="s">
         <v>56</v>
@@ -4041,24 +4185,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>333</v>
+        <v>347</v>
       </c>
       <c r="D67" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="E67" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F67" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="G67" t="s">
-        <v>345</v>
+        <v>359</v>
       </c>
       <c r="I67" t="s">
         <v>56</v>
@@ -4073,24 +4217,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="D68" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
       <c r="E68" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F68" t="s">
-        <v>356</v>
+        <v>371</v>
       </c>
       <c r="G68" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="I68" t="s">
         <v>56</v>
@@ -4105,24 +4249,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>365</v>
+        <v>332</v>
       </c>
       <c r="D69" t="s">
-        <v>368</v>
+        <v>336</v>
       </c>
       <c r="E69" t="s">
         <v>225</v>
       </c>
       <c r="F69" t="s">
-        <v>373</v>
+        <v>340</v>
       </c>
       <c r="G69" t="s">
-        <v>377</v>
+        <v>344</v>
       </c>
       <c r="I69" t="s">
         <v>56</v>
@@ -4137,713 +4281,1161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>8</v>
       </c>
       <c r="C70" t="s">
+        <v>348</v>
+      </c>
+      <c r="D70" t="s">
+        <v>352</v>
+      </c>
+      <c r="E70" t="s">
+        <v>225</v>
+      </c>
+      <c r="F70" t="s">
+        <v>355</v>
+      </c>
+      <c r="G70" t="s">
+        <v>360</v>
+      </c>
+      <c r="I70" t="s">
+        <v>56</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" t="s">
+        <v>364</v>
+      </c>
+      <c r="D71" t="s">
+        <v>367</v>
+      </c>
+      <c r="E71" t="s">
+        <v>225</v>
+      </c>
+      <c r="F71" t="s">
+        <v>372</v>
+      </c>
+      <c r="G71" t="s">
+        <v>376</v>
+      </c>
+      <c r="I71" t="s">
+        <v>56</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" t="s">
+        <v>333</v>
+      </c>
+      <c r="D72" t="s">
+        <v>337</v>
+      </c>
+      <c r="E72" t="s">
+        <v>225</v>
+      </c>
+      <c r="F72" t="s">
+        <v>341</v>
+      </c>
+      <c r="G72" t="s">
+        <v>345</v>
+      </c>
+      <c r="I72" t="s">
+        <v>56</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>349</v>
+      </c>
+      <c r="D73" t="s">
+        <v>353</v>
+      </c>
+      <c r="E73" t="s">
+        <v>225</v>
+      </c>
+      <c r="F73" t="s">
+        <v>356</v>
+      </c>
+      <c r="G73" t="s">
+        <v>361</v>
+      </c>
+      <c r="I73" t="s">
+        <v>56</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73">
+        <v>1</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" t="s">
+        <v>365</v>
+      </c>
+      <c r="D74" t="s">
+        <v>368</v>
+      </c>
+      <c r="E74" t="s">
+        <v>225</v>
+      </c>
+      <c r="F74" t="s">
+        <v>373</v>
+      </c>
+      <c r="G74" t="s">
+        <v>377</v>
+      </c>
+      <c r="I74" t="s">
+        <v>56</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
         <v>85</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D75" t="s">
         <v>81</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E75" t="s">
         <v>222</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F75" t="s">
         <v>82</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G75" t="s">
         <v>83</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I75" t="s">
         <v>84</v>
       </c>
-      <c r="J70">
-        <v>1</v>
-      </c>
-      <c r="K70">
-        <v>1</v>
-      </c>
-      <c r="L70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>8</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="K75">
+        <v>1</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
         <v>86</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D76" t="s">
         <v>87</v>
-      </c>
-      <c r="E71" t="s">
-        <v>223</v>
-      </c>
-      <c r="F71" t="s">
-        <v>88</v>
-      </c>
-      <c r="G71" t="s">
-        <v>89</v>
-      </c>
-      <c r="I71" t="s">
-        <v>84</v>
-      </c>
-      <c r="J71">
-        <v>1</v>
-      </c>
-      <c r="K71">
-        <v>1</v>
-      </c>
-      <c r="L71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>8</v>
-      </c>
-      <c r="C72" t="s">
-        <v>97</v>
-      </c>
-      <c r="D72" t="s">
-        <v>98</v>
-      </c>
-      <c r="E72" t="s">
-        <v>34</v>
-      </c>
-      <c r="F72" t="s">
-        <v>99</v>
-      </c>
-      <c r="G72" t="s">
-        <v>100</v>
-      </c>
-      <c r="I72" t="s">
-        <v>84</v>
-      </c>
-      <c r="J72">
-        <v>1</v>
-      </c>
-      <c r="K72">
-        <v>1</v>
-      </c>
-      <c r="L72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" t="s">
-        <v>101</v>
-      </c>
-      <c r="D73" t="s">
-        <v>102</v>
-      </c>
-      <c r="E73" t="s">
-        <v>34</v>
-      </c>
-      <c r="F73" t="s">
-        <v>103</v>
-      </c>
-      <c r="G73" t="s">
-        <v>104</v>
-      </c>
-      <c r="I73" t="s">
-        <v>84</v>
-      </c>
-      <c r="J73">
-        <v>1</v>
-      </c>
-      <c r="K73">
-        <v>1</v>
-      </c>
-      <c r="L73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" t="s">
-        <v>109</v>
-      </c>
-      <c r="D74" t="s">
-        <v>110</v>
-      </c>
-      <c r="E74" t="s">
-        <v>223</v>
-      </c>
-      <c r="F74" t="s">
-        <v>111</v>
-      </c>
-      <c r="G74" t="s">
-        <v>112</v>
-      </c>
-      <c r="I74" t="s">
-        <v>113</v>
-      </c>
-      <c r="J74">
-        <v>1</v>
-      </c>
-      <c r="K74">
-        <v>1</v>
-      </c>
-      <c r="L74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>8</v>
-      </c>
-      <c r="C75" t="s">
-        <v>114</v>
-      </c>
-      <c r="D75" t="s">
-        <v>115</v>
-      </c>
-      <c r="E75" t="s">
-        <v>223</v>
-      </c>
-      <c r="F75" t="s">
-        <v>116</v>
-      </c>
-      <c r="G75" t="s">
-        <v>117</v>
-      </c>
-      <c r="I75" t="s">
-        <v>113</v>
-      </c>
-      <c r="J75">
-        <v>1</v>
-      </c>
-      <c r="K75">
-        <v>1</v>
-      </c>
-      <c r="L75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>8</v>
-      </c>
-      <c r="C76" t="s">
-        <v>118</v>
-      </c>
-      <c r="D76" t="s">
-        <v>119</v>
       </c>
       <c r="E76" t="s">
         <v>223</v>
       </c>
       <c r="F76" t="s">
+        <v>88</v>
+      </c>
+      <c r="G76" t="s">
+        <v>89</v>
+      </c>
+      <c r="I76" t="s">
+        <v>84</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76">
+        <v>1</v>
+      </c>
+      <c r="L76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>97</v>
+      </c>
+      <c r="D77" t="s">
+        <v>98</v>
+      </c>
+      <c r="E77" t="s">
+        <v>34</v>
+      </c>
+      <c r="F77" t="s">
+        <v>99</v>
+      </c>
+      <c r="G77" t="s">
+        <v>100</v>
+      </c>
+      <c r="I77" t="s">
+        <v>84</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77">
+        <v>1</v>
+      </c>
+      <c r="L77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>101</v>
+      </c>
+      <c r="D78" t="s">
+        <v>102</v>
+      </c>
+      <c r="E78" t="s">
+        <v>34</v>
+      </c>
+      <c r="F78" t="s">
+        <v>103</v>
+      </c>
+      <c r="G78" t="s">
+        <v>104</v>
+      </c>
+      <c r="I78" t="s">
+        <v>84</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="K78">
+        <v>1</v>
+      </c>
+      <c r="L78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
+        <v>109</v>
+      </c>
+      <c r="D79" t="s">
+        <v>110</v>
+      </c>
+      <c r="E79" t="s">
+        <v>223</v>
+      </c>
+      <c r="F79" t="s">
+        <v>111</v>
+      </c>
+      <c r="G79" t="s">
+        <v>112</v>
+      </c>
+      <c r="I79" t="s">
+        <v>113</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>114</v>
+      </c>
+      <c r="D80" t="s">
+        <v>115</v>
+      </c>
+      <c r="E80" t="s">
+        <v>223</v>
+      </c>
+      <c r="F80" t="s">
+        <v>116</v>
+      </c>
+      <c r="G80" t="s">
+        <v>117</v>
+      </c>
+      <c r="I80" t="s">
+        <v>113</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" t="s">
+        <v>118</v>
+      </c>
+      <c r="D81" t="s">
+        <v>119</v>
+      </c>
+      <c r="E81" t="s">
+        <v>223</v>
+      </c>
+      <c r="F81" t="s">
         <v>120</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G81" t="s">
         <v>125</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I81" t="s">
         <v>113</v>
       </c>
-      <c r="J76">
-        <v>1</v>
-      </c>
-      <c r="K76">
-        <v>1</v>
-      </c>
-      <c r="L76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
         <v>121</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D82" t="s">
         <v>122</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E82" t="s">
         <v>223</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F82" t="s">
         <v>123</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G82" t="s">
         <v>124</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I82" t="s">
         <v>113</v>
       </c>
-      <c r="J77">
-        <v>1</v>
-      </c>
-      <c r="K77">
-        <v>1</v>
-      </c>
-      <c r="L77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
         <v>174</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D83" t="s">
         <v>173</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E83" t="s">
         <v>175</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F83" t="s">
         <v>176</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G83" t="s">
         <v>177</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I83" t="s">
         <v>178</v>
       </c>
-      <c r="J78">
-        <v>1</v>
-      </c>
-      <c r="K78">
-        <v>1</v>
-      </c>
-      <c r="L78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>1</v>
+      </c>
+      <c r="L83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" t="s">
         <v>157</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D84" t="s">
         <v>158</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E84" t="s">
         <v>160</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F84" t="s">
         <v>159</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G84" t="s">
         <v>171</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I84" t="s">
         <v>161</v>
       </c>
-      <c r="J79">
-        <v>1</v>
-      </c>
-      <c r="K79">
-        <v>1</v>
-      </c>
-      <c r="L79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+      <c r="J84">
+        <v>1</v>
+      </c>
+      <c r="K84">
+        <v>1</v>
+      </c>
+      <c r="L84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" t="s">
+        <v>400</v>
+      </c>
+      <c r="D85" t="s">
+        <v>401</v>
+      </c>
+      <c r="E85" t="s">
+        <v>402</v>
+      </c>
+      <c r="F85" t="s">
+        <v>403</v>
+      </c>
+      <c r="G85" t="s">
+        <v>404</v>
+      </c>
+      <c r="I85" t="s">
+        <v>113</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85">
+        <v>1</v>
+      </c>
+      <c r="L85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" t="s">
+        <v>405</v>
+      </c>
+      <c r="D86" t="s">
+        <v>406</v>
+      </c>
+      <c r="E86" t="s">
+        <v>407</v>
+      </c>
+      <c r="F86" t="s">
+        <v>408</v>
+      </c>
+      <c r="G86" t="s">
+        <v>409</v>
+      </c>
+      <c r="I86" t="s">
+        <v>58</v>
+      </c>
+      <c r="J86">
+        <v>1</v>
+      </c>
+      <c r="K86">
+        <v>1</v>
+      </c>
+      <c r="L86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" t="s">
+        <v>410</v>
+      </c>
+      <c r="D87" t="s">
+        <v>411</v>
+      </c>
+      <c r="E87" t="s">
+        <v>402</v>
+      </c>
+      <c r="F87" t="s">
+        <v>412</v>
+      </c>
+      <c r="G87" t="s">
+        <v>413</v>
+      </c>
+      <c r="I87" t="s">
+        <v>58</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+      <c r="K87">
+        <v>1</v>
+      </c>
+      <c r="L87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>5</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C88" t="s">
         <v>167</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D88" t="s">
         <v>131</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E88" t="s">
         <v>59</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F88" t="s">
         <v>132</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G88" t="s">
         <v>133</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I88" t="s">
         <v>134</v>
       </c>
-      <c r="J80">
-        <v>1</v>
-      </c>
-      <c r="K80">
-        <v>1</v>
-      </c>
-      <c r="L80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="L88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>5</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C89" t="s">
         <v>77</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D89" t="s">
         <v>63</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E89" t="s">
         <v>182</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F89" t="s">
         <v>67</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G89" t="s">
         <v>50</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I89" t="s">
         <v>71</v>
       </c>
-      <c r="J81">
-        <v>1</v>
-      </c>
-      <c r="K81">
-        <v>1</v>
-      </c>
-      <c r="L81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+      <c r="J89">
+        <v>1</v>
+      </c>
+      <c r="K89">
+        <v>1</v>
+      </c>
+      <c r="L89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>5</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C90" t="s">
         <v>73</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D90" t="s">
         <v>92</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E90" t="s">
         <v>49</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F90" t="s">
         <v>94</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G90" t="s">
         <v>169</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I90" t="s">
         <v>96</v>
       </c>
-      <c r="J82">
-        <v>1</v>
-      </c>
-      <c r="K82">
-        <v>1</v>
-      </c>
-      <c r="L82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="K90">
+        <v>1</v>
+      </c>
+      <c r="L90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>5</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C91" t="s">
         <v>90</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D91" t="s">
         <v>93</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E91" t="s">
         <v>49</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F91" t="s">
         <v>95</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G91" t="s">
         <v>170</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I91" t="s">
         <v>96</v>
       </c>
-      <c r="J83">
-        <v>1</v>
-      </c>
-      <c r="K83">
-        <v>1</v>
-      </c>
-      <c r="L83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+      <c r="J91">
+        <v>1</v>
+      </c>
+      <c r="K91">
+        <v>1</v>
+      </c>
+      <c r="L91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>5</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C92" t="s">
         <v>91</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D92" t="s">
         <v>78</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E92" t="s">
         <v>49</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F92" t="s">
         <v>79</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G92" t="s">
         <v>80</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I92" t="s">
         <v>96</v>
       </c>
-      <c r="J84">
-        <v>1</v>
-      </c>
-      <c r="K84">
-        <v>1</v>
-      </c>
-      <c r="L84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+      <c r="J92">
+        <v>1</v>
+      </c>
+      <c r="K92">
+        <v>1</v>
+      </c>
+      <c r="L92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>5</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C93" t="s">
         <v>105</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D93" t="s">
         <v>106</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E93" t="s">
         <v>49</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F93" t="s">
         <v>107</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G93" t="s">
         <v>108</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I93" t="s">
         <v>96</v>
       </c>
-      <c r="J85">
-        <v>1</v>
-      </c>
-      <c r="K85">
-        <v>1</v>
-      </c>
-      <c r="L85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+      <c r="J93">
+        <v>1</v>
+      </c>
+      <c r="K93">
+        <v>1</v>
+      </c>
+      <c r="L93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>5</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C94" t="s">
         <v>378</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D94" t="s">
         <v>379</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E94" t="s">
         <v>34</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F94" t="s">
         <v>380</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G94" t="s">
         <v>381</v>
       </c>
-      <c r="I86" t="s">
+      <c r="I94" t="s">
         <v>72</v>
       </c>
-      <c r="J86">
-        <v>1</v>
-      </c>
-      <c r="K86">
-        <v>1</v>
-      </c>
-      <c r="L86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+      <c r="J94">
+        <v>1</v>
+      </c>
+      <c r="K94">
+        <v>1</v>
+      </c>
+      <c r="L94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>5</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C95" t="s">
         <v>162</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D95" t="s">
         <v>163</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E95" t="s">
         <v>164</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F95" t="s">
         <v>165</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G95" t="s">
         <v>168</v>
       </c>
-      <c r="I87" t="s">
+      <c r="I95" t="s">
         <v>166</v>
       </c>
-      <c r="J87">
-        <v>1</v>
-      </c>
-      <c r="K87">
-        <v>1</v>
-      </c>
-      <c r="L87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E149" s="1"/>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A285" t="s">
-        <v>14</v>
-      </c>
-      <c r="C285" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A286" t="s">
-        <v>8</v>
-      </c>
-      <c r="C286" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A287" t="s">
-        <v>8</v>
-      </c>
-      <c r="C287" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A288" t="s">
-        <v>8</v>
-      </c>
-      <c r="C288" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A289" t="s">
-        <v>6</v>
-      </c>
-      <c r="C289" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A290" t="s">
-        <v>7</v>
-      </c>
-      <c r="C290" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A291" t="s">
-        <v>6</v>
-      </c>
-      <c r="C291" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A292" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="J95">
+        <v>1</v>
+      </c>
+      <c r="K95">
+        <v>1</v>
+      </c>
+      <c r="L95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" t="s">
+        <v>431</v>
+      </c>
+      <c r="D96" t="s">
+        <v>414</v>
+      </c>
+      <c r="E96" t="s">
+        <v>415</v>
+      </c>
+      <c r="F96" t="s">
+        <v>416</v>
+      </c>
+      <c r="G96" t="s">
+        <v>417</v>
+      </c>
+      <c r="I96" t="s">
+        <v>58</v>
+      </c>
+      <c r="J96">
+        <v>1</v>
+      </c>
+      <c r="K96">
+        <v>1</v>
+      </c>
+      <c r="L96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" t="s">
+        <v>432</v>
+      </c>
+      <c r="D97" t="s">
+        <v>418</v>
+      </c>
+      <c r="E97" t="s">
+        <v>415</v>
+      </c>
+      <c r="F97" t="s">
+        <v>419</v>
+      </c>
+      <c r="G97" t="s">
+        <v>420</v>
+      </c>
+      <c r="I97" t="s">
+        <v>58</v>
+      </c>
+      <c r="J97">
+        <v>1</v>
+      </c>
+      <c r="K97">
+        <v>1</v>
+      </c>
+      <c r="L97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" t="s">
+        <v>433</v>
+      </c>
+      <c r="D98" t="s">
+        <v>421</v>
+      </c>
+      <c r="E98" t="s">
+        <v>422</v>
+      </c>
+      <c r="F98" t="s">
+        <v>423</v>
+      </c>
+      <c r="G98" t="s">
+        <v>424</v>
+      </c>
+      <c r="I98" t="s">
+        <v>58</v>
+      </c>
+      <c r="J98">
+        <v>1</v>
+      </c>
+      <c r="K98">
+        <v>1</v>
+      </c>
+      <c r="L98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" t="s">
+        <v>434</v>
+      </c>
+      <c r="D99" t="s">
+        <v>425</v>
+      </c>
+      <c r="E99" t="s">
+        <v>422</v>
+      </c>
+      <c r="F99" t="s">
+        <v>426</v>
+      </c>
+      <c r="G99" t="s">
+        <v>424</v>
+      </c>
+      <c r="I99" t="s">
+        <v>58</v>
+      </c>
+      <c r="J99">
+        <v>1</v>
+      </c>
+      <c r="K99">
+        <v>1</v>
+      </c>
+      <c r="L99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>435</v>
+      </c>
+      <c r="D100" t="s">
+        <v>427</v>
+      </c>
+      <c r="E100" t="s">
+        <v>415</v>
+      </c>
+      <c r="F100" t="s">
+        <v>428</v>
+      </c>
+      <c r="G100" t="s">
+        <v>424</v>
+      </c>
+      <c r="I100" t="s">
+        <v>58</v>
+      </c>
+      <c r="J100">
+        <v>1</v>
+      </c>
+      <c r="K100">
+        <v>1</v>
+      </c>
+      <c r="L100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
+        <v>436</v>
+      </c>
+      <c r="D101" t="s">
+        <v>429</v>
+      </c>
+      <c r="E101" t="s">
+        <v>415</v>
+      </c>
+      <c r="F101" t="s">
+        <v>430</v>
+      </c>
+      <c r="G101" t="s">
+        <v>424</v>
+      </c>
+      <c r="I101" t="s">
+        <v>58</v>
+      </c>
+      <c r="J101">
+        <v>1</v>
+      </c>
+      <c r="K101">
+        <v>1</v>
+      </c>
+      <c r="L101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E157" s="1"/>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C293" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="C294" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="C295" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="C296" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="C297" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="C298" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="C299" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>